<commit_message>
added liu, mdh, his 2020 data. Some more corrections.
</commit_message>
<xml_diff>
--- a/data/liu/original_data/2019_liu_corrections.xlsx
+++ b/data/liu/original_data/2019_liu_corrections.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>institution</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Elsevier</t>
+  </si>
+  <si>
+    <t>10.21037/hbsn.2019.10.36</t>
+  </si>
+  <si>
+    <t>AME Publishing Company</t>
   </si>
 </sst>
 </file>
@@ -155,9 +161,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -558,6 +567,26 @@
         <v>19</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C5">
+        <v>13708</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>